<commit_message>
Ajustes Sonhe+Alto: DB isolado fM71 e nova tela de login
</commit_message>
<xml_diff>
--- a/Projeto21/Projeto21_com_frequencia_de_todas_areas_com_manual.xlsx
+++ b/Projeto21/Projeto21_com_frequencia_de_todas_areas_com_manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wanderley\Apps\escola_no_ar_site\Projeto21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3ED076-CFB2-48FF-BCF5-BA3477E18FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0B7720-D5B5-4A74-9F02-9EE78D422DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo &amp; Instruções" sheetId="1" r:id="rId1"/>
@@ -1686,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="I1:J1"/>
     </sheetView>
   </sheetViews>
@@ -3495,7 +3495,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
@@ -5351,7 +5351,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5744,21 +5744,21 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="M8" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>EuA015-1d0d</v>
+        <v>EuA015-1d1d</v>
       </c>
       <c r="N8" s="9">
         <v>3</v>
       </c>
       <c r="O8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Uma vez por dia por um período de 0 dias</v>
+        <v>Pelo menos uma vez</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -7221,9 +7221,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="A39:XFD46"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8981,8 +8981,8 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD50"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10663,16 +10663,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:F1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="7" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" style="10" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" style="10" bestFit="1" customWidth="1"/>

</xml_diff>